<commit_message>
modularised and added multifilter
</commit_message>
<xml_diff>
--- a/coauthor-analyses/analysis_results.xlsx
+++ b/coauthor-analyses/analysis_results.xlsx
@@ -7,14 +7,16 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="organisations" sheetId="1" r:id="rId1"/>
+    <sheet name="author_organisations_all" sheetId="1" r:id="rId1"/>
+    <sheet name="author_organisations_cleaned" sheetId="2" r:id="rId2"/>
+    <sheet name="author_organisations_uni" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="875">
   <si>
     <t>organisation</t>
   </si>
@@ -2725,35 +2727,83 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>234725</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>18311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="author_organisations_uni.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="author_organisations_cleaned.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1828800" y="11620500"/>
+          <a:off x="1828800" y="190500"/>
+          <a:ext cx="14255525" cy="11448311"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>234725</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>18311</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="author_organisations_uni.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="190500"/>
           <a:ext cx="14255525" cy="11448311"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10053,4 +10103,4016 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B264"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>190</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>194</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>211</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>224</v>
+      </c>
+      <c r="B51">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>225</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>228</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>233</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>235</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>238</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>239</v>
+      </c>
+      <c r="B57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>240</v>
+      </c>
+      <c r="B58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>241</v>
+      </c>
+      <c r="B59">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>250</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>264</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>266</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>273</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>274</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>277</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>280</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>285</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>288</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>289</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>292</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>294</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>303</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>309</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>311</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>312</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>314</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>319</v>
+      </c>
+      <c r="B80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>320</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>323</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>324</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>326</v>
+      </c>
+      <c r="B84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>328</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>329</v>
+      </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>333</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>337</v>
+      </c>
+      <c r="B88">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>341</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>342</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>343</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>345</v>
+      </c>
+      <c r="B92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>346</v>
+      </c>
+      <c r="B93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>349</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>351</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>356</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>365</v>
+      </c>
+      <c r="B97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>369</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>370</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>378</v>
+      </c>
+      <c r="B100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>379</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>384</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>385</v>
+      </c>
+      <c r="B103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>389</v>
+      </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>390</v>
+      </c>
+      <c r="B105">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>394</v>
+      </c>
+      <c r="B106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>396</v>
+      </c>
+      <c r="B107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>397</v>
+      </c>
+      <c r="B108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>400</v>
+      </c>
+      <c r="B109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>401</v>
+      </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>407</v>
+      </c>
+      <c r="B111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>411</v>
+      </c>
+      <c r="B112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>413</v>
+      </c>
+      <c r="B113">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>423</v>
+      </c>
+      <c r="B114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>424</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>426</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>427</v>
+      </c>
+      <c r="B117">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>430</v>
+      </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>433</v>
+      </c>
+      <c r="B119">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>434</v>
+      </c>
+      <c r="B120">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>439</v>
+      </c>
+      <c r="B121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>450</v>
+      </c>
+      <c r="B122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>454</v>
+      </c>
+      <c r="B123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>456</v>
+      </c>
+      <c r="B124">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>458</v>
+      </c>
+      <c r="B125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>459</v>
+      </c>
+      <c r="B126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>460</v>
+      </c>
+      <c r="B127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>463</v>
+      </c>
+      <c r="B128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>466</v>
+      </c>
+      <c r="B129">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>467</v>
+      </c>
+      <c r="B130">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>475</v>
+      </c>
+      <c r="B131">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>476</v>
+      </c>
+      <c r="B132">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>477</v>
+      </c>
+      <c r="B133">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>478</v>
+      </c>
+      <c r="B134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>479</v>
+      </c>
+      <c r="B135">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>484</v>
+      </c>
+      <c r="B136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>487</v>
+      </c>
+      <c r="B137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>492</v>
+      </c>
+      <c r="B138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>497</v>
+      </c>
+      <c r="B139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>499</v>
+      </c>
+      <c r="B140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>502</v>
+      </c>
+      <c r="B141">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>505</v>
+      </c>
+      <c r="B142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>506</v>
+      </c>
+      <c r="B143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>509</v>
+      </c>
+      <c r="B144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>510</v>
+      </c>
+      <c r="B145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>512</v>
+      </c>
+      <c r="B146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>513</v>
+      </c>
+      <c r="B147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>524</v>
+      </c>
+      <c r="B148">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>525</v>
+      </c>
+      <c r="B149">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>526</v>
+      </c>
+      <c r="B150">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>529</v>
+      </c>
+      <c r="B151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>533</v>
+      </c>
+      <c r="B152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>535</v>
+      </c>
+      <c r="B153">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>537</v>
+      </c>
+      <c r="B154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>539</v>
+      </c>
+      <c r="B155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>543</v>
+      </c>
+      <c r="B156">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>544</v>
+      </c>
+      <c r="B157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>549</v>
+      </c>
+      <c r="B158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>553</v>
+      </c>
+      <c r="B159">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>575</v>
+      </c>
+      <c r="B160">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>584</v>
+      </c>
+      <c r="B161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>591</v>
+      </c>
+      <c r="B162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>593</v>
+      </c>
+      <c r="B163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>599</v>
+      </c>
+      <c r="B164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>600</v>
+      </c>
+      <c r="B165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>604</v>
+      </c>
+      <c r="B166">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>606</v>
+      </c>
+      <c r="B167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>609</v>
+      </c>
+      <c r="B168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>610</v>
+      </c>
+      <c r="B169">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>612</v>
+      </c>
+      <c r="B170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>617</v>
+      </c>
+      <c r="B171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>626</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>627</v>
+      </c>
+      <c r="B173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>628</v>
+      </c>
+      <c r="B174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>630</v>
+      </c>
+      <c r="B175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>632</v>
+      </c>
+      <c r="B176">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>634</v>
+      </c>
+      <c r="B177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>637</v>
+      </c>
+      <c r="B178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>639</v>
+      </c>
+      <c r="B179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>640</v>
+      </c>
+      <c r="B180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>641</v>
+      </c>
+      <c r="B181">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>642</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>643</v>
+      </c>
+      <c r="B183">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>645</v>
+      </c>
+      <c r="B184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>650</v>
+      </c>
+      <c r="B185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>652</v>
+      </c>
+      <c r="B186">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>654</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>662</v>
+      </c>
+      <c r="B188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>664</v>
+      </c>
+      <c r="B189">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>670</v>
+      </c>
+      <c r="B190">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>679</v>
+      </c>
+      <c r="B191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>682</v>
+      </c>
+      <c r="B192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>683</v>
+      </c>
+      <c r="B193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>685</v>
+      </c>
+      <c r="B194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>687</v>
+      </c>
+      <c r="B195">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>691</v>
+      </c>
+      <c r="B196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>695</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>698</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>703</v>
+      </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>705</v>
+      </c>
+      <c r="B200">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>707</v>
+      </c>
+      <c r="B201">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>708</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>709</v>
+      </c>
+      <c r="B203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>712</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>716</v>
+      </c>
+      <c r="B205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>717</v>
+      </c>
+      <c r="B206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>722</v>
+      </c>
+      <c r="B207">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>728</v>
+      </c>
+      <c r="B208">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>730</v>
+      </c>
+      <c r="B209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>731</v>
+      </c>
+      <c r="B210">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>733</v>
+      </c>
+      <c r="B211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>735</v>
+      </c>
+      <c r="B212">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>736</v>
+      </c>
+      <c r="B213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>740</v>
+      </c>
+      <c r="B214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>741</v>
+      </c>
+      <c r="B215">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>745</v>
+      </c>
+      <c r="B216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>748</v>
+      </c>
+      <c r="B217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>750</v>
+      </c>
+      <c r="B218">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>751</v>
+      </c>
+      <c r="B219">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>753</v>
+      </c>
+      <c r="B220">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>754</v>
+      </c>
+      <c r="B221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>755</v>
+      </c>
+      <c r="B222">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>756</v>
+      </c>
+      <c r="B223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>758</v>
+      </c>
+      <c r="B224">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>762</v>
+      </c>
+      <c r="B225">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>765</v>
+      </c>
+      <c r="B226">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>766</v>
+      </c>
+      <c r="B227">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>768</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>770</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>771</v>
+      </c>
+      <c r="B230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>772</v>
+      </c>
+      <c r="B231">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>773</v>
+      </c>
+      <c r="B232">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>774</v>
+      </c>
+      <c r="B233">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>775</v>
+      </c>
+      <c r="B234">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>779</v>
+      </c>
+      <c r="B235">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>782</v>
+      </c>
+      <c r="B236">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>784</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>786</v>
+      </c>
+      <c r="B238">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>789</v>
+      </c>
+      <c r="B239">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>790</v>
+      </c>
+      <c r="B240">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>792</v>
+      </c>
+      <c r="B241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>793</v>
+      </c>
+      <c r="B242">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>794</v>
+      </c>
+      <c r="B243">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>798</v>
+      </c>
+      <c r="B244">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>801</v>
+      </c>
+      <c r="B245">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>802</v>
+      </c>
+      <c r="B246">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>806</v>
+      </c>
+      <c r="B247">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>815</v>
+      </c>
+      <c r="B248">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>818</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>821</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>824</v>
+      </c>
+      <c r="B251">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>836</v>
+      </c>
+      <c r="B252">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>838</v>
+      </c>
+      <c r="B253">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>841</v>
+      </c>
+      <c r="B254">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>842</v>
+      </c>
+      <c r="B255">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>848</v>
+      </c>
+      <c r="B256">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>852</v>
+      </c>
+      <c r="B257">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>853</v>
+      </c>
+      <c r="B258">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>857</v>
+      </c>
+      <c r="B259">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>862</v>
+      </c>
+      <c r="B260">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>865</v>
+      </c>
+      <c r="B261">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>870</v>
+      </c>
+      <c r="B262">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>873</v>
+      </c>
+      <c r="B263">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>874</v>
+      </c>
+      <c r="B264">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B234"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>232</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>274</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>279</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>282</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>289</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>301</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>303</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>304</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>311</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>315</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>319</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>346</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>372</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>374</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>377</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>378</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>379</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>381</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>389</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>391</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>392</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>393</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>400</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>416</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>425</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>427</v>
+      </c>
+      <c r="B56">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>428</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>429</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>434</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>439</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>440</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>441</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>450</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>452</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>456</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>457</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>465</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>471</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>473</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>480</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>484</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>486</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>488</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>498</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>499</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>500</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>508</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>509</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>510</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>513</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>519</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>520</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>529</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>542</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>543</v>
+      </c>
+      <c r="B85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>544</v>
+      </c>
+      <c r="B86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>546</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>549</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>552</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>553</v>
+      </c>
+      <c r="B90">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>562</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>565</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>590</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>604</v>
+      </c>
+      <c r="B94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>610</v>
+      </c>
+      <c r="B95">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>617</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>623</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>637</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>640</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>641</v>
+      </c>
+      <c r="B100">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>642</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>643</v>
+      </c>
+      <c r="B102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>646</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>648</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>667</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>668</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>669</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>672</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>677</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>678</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>700</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>701</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>702</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>703</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>704</v>
+      </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>705</v>
+      </c>
+      <c r="B116">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>706</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>707</v>
+      </c>
+      <c r="B118">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>708</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>709</v>
+      </c>
+      <c r="B120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>710</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>711</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>712</v>
+      </c>
+      <c r="B123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>713</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>714</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>715</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>716</v>
+      </c>
+      <c r="B127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>717</v>
+      </c>
+      <c r="B128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>718</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>719</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>720</v>
+      </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>721</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>722</v>
+      </c>
+      <c r="B133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>723</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>724</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>725</v>
+      </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>726</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>727</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>728</v>
+      </c>
+      <c r="B139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>729</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>730</v>
+      </c>
+      <c r="B141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>731</v>
+      </c>
+      <c r="B142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>732</v>
+      </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>733</v>
+      </c>
+      <c r="B144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>734</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>735</v>
+      </c>
+      <c r="B146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>736</v>
+      </c>
+      <c r="B147">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>737</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>738</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>739</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>740</v>
+      </c>
+      <c r="B151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>741</v>
+      </c>
+      <c r="B152">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>742</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>743</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>744</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>745</v>
+      </c>
+      <c r="B156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>746</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>747</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>748</v>
+      </c>
+      <c r="B159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>749</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>750</v>
+      </c>
+      <c r="B161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>751</v>
+      </c>
+      <c r="B162">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>752</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>753</v>
+      </c>
+      <c r="B164">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>754</v>
+      </c>
+      <c r="B165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>755</v>
+      </c>
+      <c r="B166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>756</v>
+      </c>
+      <c r="B167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>757</v>
+      </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>758</v>
+      </c>
+      <c r="B169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>759</v>
+      </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>760</v>
+      </c>
+      <c r="B171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>761</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>762</v>
+      </c>
+      <c r="B173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>763</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>764</v>
+      </c>
+      <c r="B175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>765</v>
+      </c>
+      <c r="B176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>766</v>
+      </c>
+      <c r="B177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>767</v>
+      </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>768</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>769</v>
+      </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>770</v>
+      </c>
+      <c r="B181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>771</v>
+      </c>
+      <c r="B182">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>772</v>
+      </c>
+      <c r="B183">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>773</v>
+      </c>
+      <c r="B184">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>774</v>
+      </c>
+      <c r="B185">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>775</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>776</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>777</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>778</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>779</v>
+      </c>
+      <c r="B190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>780</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>781</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>782</v>
+      </c>
+      <c r="B193">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>783</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>784</v>
+      </c>
+      <c r="B195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>785</v>
+      </c>
+      <c r="B196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>786</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>787</v>
+      </c>
+      <c r="B198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>788</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>789</v>
+      </c>
+      <c r="B200">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>790</v>
+      </c>
+      <c r="B201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>791</v>
+      </c>
+      <c r="B202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>792</v>
+      </c>
+      <c r="B203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>793</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>794</v>
+      </c>
+      <c r="B205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>795</v>
+      </c>
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>796</v>
+      </c>
+      <c r="B207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>797</v>
+      </c>
+      <c r="B208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>798</v>
+      </c>
+      <c r="B209">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>799</v>
+      </c>
+      <c r="B210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>800</v>
+      </c>
+      <c r="B211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>801</v>
+      </c>
+      <c r="B212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>802</v>
+      </c>
+      <c r="B213">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>803</v>
+      </c>
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>804</v>
+      </c>
+      <c r="B215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>805</v>
+      </c>
+      <c r="B216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>806</v>
+      </c>
+      <c r="B217">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>807</v>
+      </c>
+      <c r="B218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>808</v>
+      </c>
+      <c r="B219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>809</v>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>810</v>
+      </c>
+      <c r="B221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>821</v>
+      </c>
+      <c r="B222">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>824</v>
+      </c>
+      <c r="B223">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>828</v>
+      </c>
+      <c r="B224">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>829</v>
+      </c>
+      <c r="B225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>833</v>
+      </c>
+      <c r="B226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>835</v>
+      </c>
+      <c r="B227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>842</v>
+      </c>
+      <c r="B228">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>843</v>
+      </c>
+      <c r="B229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>845</v>
+      </c>
+      <c r="B230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>854</v>
+      </c>
+      <c r="B231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>857</v>
+      </c>
+      <c r="B232">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>872</v>
+      </c>
+      <c r="B233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>874</v>
+      </c>
+      <c r="B234">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>